<commit_message>
Built site for robonomistClient: 2.1.2@71ec54a
</commit_message>
<xml_diff>
--- a/reference/figures/export.xlsx
+++ b/reference/figures/export.xlsx
@@ -361,7 +361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1898,6 +1898,63 @@
         <v>10.2</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Construction confidence indicator (5%)</t>
+        </is>
+      </c>
+      <c r="B81" s="2">
+        <v>44409</v>
+      </c>
+      <c r="C81">
+        <v>5.5</v>
+      </c>
+      <c r="D81">
+        <v>2.3</v>
+      </c>
+      <c r="E81">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Construction confidence indicator (5%)</t>
+        </is>
+      </c>
+      <c r="B82" s="2">
+        <v>44440</v>
+      </c>
+      <c r="C82">
+        <v>8.6</v>
+      </c>
+      <c r="D82">
+        <v>4.5</v>
+      </c>
+      <c r="E82">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Construction confidence indicator (5%)</t>
+        </is>
+      </c>
+      <c r="B83" s="2">
+        <v>44470</v>
+      </c>
+      <c r="C83">
+        <v>10.2</v>
+      </c>
+      <c r="D83">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="E83">
+        <v>16.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1905,7 +1962,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3442,6 +3499,63 @@
         <v>7.9</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Consumer confidence indicator (20%)</t>
+        </is>
+      </c>
+      <c r="B81" s="2">
+        <v>44409</v>
+      </c>
+      <c r="C81">
+        <v>-3.5</v>
+      </c>
+      <c r="D81">
+        <v>4.2</v>
+      </c>
+      <c r="E81">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Consumer confidence indicator (20%)</t>
+        </is>
+      </c>
+      <c r="B82" s="2">
+        <v>44440</v>
+      </c>
+      <c r="C82">
+        <v>-1.1</v>
+      </c>
+      <c r="D82">
+        <v>6.3</v>
+      </c>
+      <c r="E82">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Consumer confidence indicator (20%)</t>
+        </is>
+      </c>
+      <c r="B83" s="2">
+        <v>44470</v>
+      </c>
+      <c r="C83">
+        <v>-1.5</v>
+      </c>
+      <c r="D83">
+        <v>4.5</v>
+      </c>
+      <c r="E83">
+        <v>5.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3449,7 +3563,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4986,6 +5100,63 @@
         <v>28.6</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Industrial confidence indicator (40%)</t>
+        </is>
+      </c>
+      <c r="B81" s="2">
+        <v>44409</v>
+      </c>
+      <c r="C81">
+        <v>23.9</v>
+      </c>
+      <c r="D81">
+        <v>23.4</v>
+      </c>
+      <c r="E81">
+        <v>30.7</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Industrial confidence indicator (40%)</t>
+        </is>
+      </c>
+      <c r="B82" s="2">
+        <v>44440</v>
+      </c>
+      <c r="C82">
+        <v>25.6</v>
+      </c>
+      <c r="D82">
+        <v>22.3</v>
+      </c>
+      <c r="E82">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Industrial confidence indicator (40%)</t>
+        </is>
+      </c>
+      <c r="B83" s="2">
+        <v>44470</v>
+      </c>
+      <c r="C83">
+        <v>23</v>
+      </c>
+      <c r="D83">
+        <v>24</v>
+      </c>
+      <c r="E83">
+        <v>32.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4993,7 +5164,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5039,7 +5210,7 @@
         <v>42005</v>
       </c>
       <c r="C2">
-        <v>-9.300000000000001</v>
+        <v>-9.5</v>
       </c>
       <c r="D2">
         <v>-27.1</v>
@@ -5058,7 +5229,7 @@
         <v>42036</v>
       </c>
       <c r="C3">
-        <v>-8.9</v>
+        <v>-9</v>
       </c>
       <c r="D3">
         <v>-30</v>
@@ -5077,7 +5248,7 @@
         <v>42064</v>
       </c>
       <c r="C4">
-        <v>-7.7</v>
+        <v>-7.6</v>
       </c>
       <c r="D4">
         <v>-26.1</v>
@@ -5096,7 +5267,7 @@
         <v>42095</v>
       </c>
       <c r="C5">
-        <v>-6.9</v>
+        <v>-7</v>
       </c>
       <c r="D5">
         <v>-24.1</v>
@@ -5115,7 +5286,7 @@
         <v>42125</v>
       </c>
       <c r="C6">
-        <v>-5.6</v>
+        <v>-5.7</v>
       </c>
       <c r="D6">
         <v>-22.1</v>
@@ -5134,7 +5305,7 @@
         <v>42156</v>
       </c>
       <c r="C7">
-        <v>-4.9</v>
+        <v>-5</v>
       </c>
       <c r="D7">
         <v>-26.6</v>
@@ -5153,7 +5324,7 @@
         <v>42186</v>
       </c>
       <c r="C8">
-        <v>-1.3</v>
+        <v>-1.4</v>
       </c>
       <c r="D8">
         <v>-16.4</v>
@@ -5172,7 +5343,7 @@
         <v>42217</v>
       </c>
       <c r="C9">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="D9">
         <v>-13.4</v>
@@ -5419,7 +5590,7 @@
         <v>42614</v>
       </c>
       <c r="C22">
-        <v>-3.6</v>
+        <v>-3.7</v>
       </c>
       <c r="D22">
         <v>-4.1</v>
@@ -5438,7 +5609,7 @@
         <v>42644</v>
       </c>
       <c r="C23">
-        <v>-3.5</v>
+        <v>-3.6</v>
       </c>
       <c r="D23">
         <v>-2</v>
@@ -5457,7 +5628,7 @@
         <v>42675</v>
       </c>
       <c r="C24">
-        <v>-2.2</v>
+        <v>-2.3</v>
       </c>
       <c r="D24">
         <v>-8.300000000000001</v>
@@ -5476,7 +5647,7 @@
         <v>42705</v>
       </c>
       <c r="C25">
-        <v>-3.4</v>
+        <v>-3.5</v>
       </c>
       <c r="D25">
         <v>-3.9</v>
@@ -5495,7 +5666,7 @@
         <v>42736</v>
       </c>
       <c r="C26">
-        <v>-5.4</v>
+        <v>-5.5</v>
       </c>
       <c r="D26">
         <v>-8.300000000000001</v>
@@ -5552,7 +5723,7 @@
         <v>42826</v>
       </c>
       <c r="C29">
-        <v>-0.3</v>
+        <v>-0.2</v>
       </c>
       <c r="D29">
         <v>2.2</v>
@@ -5590,7 +5761,7 @@
         <v>42887</v>
       </c>
       <c r="C31">
-        <v>-1.7</v>
+        <v>-1.6</v>
       </c>
       <c r="D31">
         <v>4.6</v>
@@ -5609,7 +5780,7 @@
         <v>42917</v>
       </c>
       <c r="C32">
-        <v>-3</v>
+        <v>-2.9</v>
       </c>
       <c r="D32">
         <v>15.2</v>
@@ -6528,6 +6699,63 @@
       </c>
       <c r="E80">
         <v>27.4</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Retail trade confidence indicator (5%)</t>
+        </is>
+      </c>
+      <c r="B81" s="2">
+        <v>44409</v>
+      </c>
+      <c r="C81">
+        <v>0.3</v>
+      </c>
+      <c r="D81">
+        <v>7.2</v>
+      </c>
+      <c r="E81">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Retail trade confidence indicator (5%)</t>
+        </is>
+      </c>
+      <c r="B82" s="2">
+        <v>44440</v>
+      </c>
+      <c r="C82">
+        <v>0.7</v>
+      </c>
+      <c r="D82">
+        <v>5.3</v>
+      </c>
+      <c r="E82">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Retail trade confidence indicator (5%)</t>
+        </is>
+      </c>
+      <c r="B83" s="2">
+        <v>44470</v>
+      </c>
+      <c r="C83">
+        <v>-0.2</v>
+      </c>
+      <c r="D83">
+        <v>10.2</v>
+      </c>
+      <c r="E83">
+        <v>24.9</v>
       </c>
     </row>
   </sheetData>
@@ -6537,7 +6765,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8074,6 +8302,63 @@
         <v>41</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Services confidence indicator (30 %)</t>
+        </is>
+      </c>
+      <c r="B81" s="2">
+        <v>44409</v>
+      </c>
+      <c r="C81">
+        <v>21</v>
+      </c>
+      <c r="D81">
+        <v>13.5</v>
+      </c>
+      <c r="E81">
+        <v>38.1</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Services confidence indicator (30 %)</t>
+        </is>
+      </c>
+      <c r="B82" s="2">
+        <v>44440</v>
+      </c>
+      <c r="C82">
+        <v>18</v>
+      </c>
+      <c r="D82">
+        <v>15.9</v>
+      </c>
+      <c r="E82">
+        <v>38.7</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Services confidence indicator (30 %)</t>
+        </is>
+      </c>
+      <c r="B83" s="2">
+        <v>44470</v>
+      </c>
+      <c r="C83">
+        <v>19.8</v>
+      </c>
+      <c r="D83">
+        <v>19.3</v>
+      </c>
+      <c r="E83">
+        <v>42.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8081,7 +8366,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8260,7 +8545,7 @@
         <v>42217</v>
       </c>
       <c r="C9">
-        <v>106.6</v>
+        <v>106.5</v>
       </c>
       <c r="D9">
         <v>91.09999999999999</v>
@@ -9616,6 +9901,63 @@
       </c>
       <c r="E80">
         <v>123.6</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>The Economic sentiment indicator is a composite measure (average = 100)</t>
+        </is>
+      </c>
+      <c r="B81" s="2">
+        <v>44409</v>
+      </c>
+      <c r="C81">
+        <v>117.2</v>
+      </c>
+      <c r="D81">
+        <v>116.1</v>
+      </c>
+      <c r="E81">
+        <v>123.2</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>The Economic sentiment indicator is a composite measure (average = 100)</t>
+        </is>
+      </c>
+      <c r="B82" s="2">
+        <v>44440</v>
+      </c>
+      <c r="C82">
+        <v>118</v>
+      </c>
+      <c r="D82">
+        <v>116.8</v>
+      </c>
+      <c r="E82">
+        <v>121.7</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>The Economic sentiment indicator is a composite measure (average = 100)</t>
+        </is>
+      </c>
+      <c r="B83" s="2">
+        <v>44470</v>
+      </c>
+      <c r="C83">
+        <v>117.5</v>
+      </c>
+      <c r="D83">
+        <v>117</v>
+      </c>
+      <c r="E83">
+        <v>123.8</v>
       </c>
     </row>
   </sheetData>
@@ -9625,7 +9967,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11162,6 +11504,63 @@
         <v>113.5</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>The Employment expectations indicator is a composite measure (average = 100)</t>
+        </is>
+      </c>
+      <c r="B81" s="2">
+        <v>44409</v>
+      </c>
+      <c r="C81">
+        <v>113.5</v>
+      </c>
+      <c r="D81">
+        <v>111</v>
+      </c>
+      <c r="E81">
+        <v>114.5</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>The Employment expectations indicator is a composite measure (average = 100)</t>
+        </is>
+      </c>
+      <c r="B82" s="2">
+        <v>44440</v>
+      </c>
+      <c r="C82">
+        <v>114.4</v>
+      </c>
+      <c r="D82">
+        <v>116</v>
+      </c>
+      <c r="E82">
+        <v>115.7</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>The Employment expectations indicator is a composite measure (average = 100)</t>
+        </is>
+      </c>
+      <c r="B83" s="2">
+        <v>44470</v>
+      </c>
+      <c r="C83">
+        <v>112.8</v>
+      </c>
+      <c r="D83">
+        <v>117.7</v>
+      </c>
+      <c r="E83">
+        <v>119.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Built site for robonomistClient: 2.1.8@65e642f
</commit_message>
<xml_diff>
--- a/reference/figures/export.xlsx
+++ b/reference/figures/export.xlsx
@@ -361,7 +361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1955,6 +1955,63 @@
         <v>16.4</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Construction confidence indicator (5%)</t>
+        </is>
+      </c>
+      <c r="B84" s="2">
+        <v>44501</v>
+      </c>
+      <c r="C84">
+        <v>13</v>
+      </c>
+      <c r="D84">
+        <v>11.3</v>
+      </c>
+      <c r="E84">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Construction confidence indicator (5%)</t>
+        </is>
+      </c>
+      <c r="B85" s="2">
+        <v>44531</v>
+      </c>
+      <c r="C85">
+        <v>12.3</v>
+      </c>
+      <c r="D85">
+        <v>11.6</v>
+      </c>
+      <c r="E85">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Construction confidence indicator (5%)</t>
+        </is>
+      </c>
+      <c r="B86" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C86">
+        <v>10.6</v>
+      </c>
+      <c r="D86">
+        <v>8.5</v>
+      </c>
+      <c r="E86">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1962,7 +2019,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3556,6 +3613,63 @@
         <v>5.7</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Consumer confidence indicator (20%)</t>
+        </is>
+      </c>
+      <c r="B84" s="2">
+        <v>44501</v>
+      </c>
+      <c r="C84">
+        <v>-3.9</v>
+      </c>
+      <c r="D84">
+        <v>3.3</v>
+      </c>
+      <c r="E84">
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Consumer confidence indicator (20%)</t>
+        </is>
+      </c>
+      <c r="B85" s="2">
+        <v>44531</v>
+      </c>
+      <c r="C85">
+        <v>-5.8</v>
+      </c>
+      <c r="D85">
+        <v>-1.4</v>
+      </c>
+      <c r="E85">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Consumer confidence indicator (20%)</t>
+        </is>
+      </c>
+      <c r="B86" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C86">
+        <v>-4.2</v>
+      </c>
+      <c r="D86">
+        <v>-0.6</v>
+      </c>
+      <c r="E86">
+        <v>-0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3563,7 +3677,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5157,6 +5271,63 @@
         <v>32.7</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Industrial confidence indicator (40%)</t>
+        </is>
+      </c>
+      <c r="B84" s="2">
+        <v>44501</v>
+      </c>
+      <c r="C84">
+        <v>22.9</v>
+      </c>
+      <c r="D84">
+        <v>25.8</v>
+      </c>
+      <c r="E84">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Industrial confidence indicator (40%)</t>
+        </is>
+      </c>
+      <c r="B85" s="2">
+        <v>44531</v>
+      </c>
+      <c r="C85">
+        <v>25.3</v>
+      </c>
+      <c r="D85">
+        <v>19.9</v>
+      </c>
+      <c r="E85">
+        <v>32.8</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Industrial confidence indicator (40%)</t>
+        </is>
+      </c>
+      <c r="B86" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C86">
+        <v>24.2</v>
+      </c>
+      <c r="D86">
+        <v>19.2</v>
+      </c>
+      <c r="E86">
+        <v>28.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5164,7 +5335,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6758,6 +6929,63 @@
         <v>24.9</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Retail trade confidence indicator (5%)</t>
+        </is>
+      </c>
+      <c r="B84" s="2">
+        <v>44501</v>
+      </c>
+      <c r="C84">
+        <v>1.5</v>
+      </c>
+      <c r="D84">
+        <v>10.2</v>
+      </c>
+      <c r="E84">
+        <v>28.4</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Retail trade confidence indicator (5%)</t>
+        </is>
+      </c>
+      <c r="B85" s="2">
+        <v>44531</v>
+      </c>
+      <c r="C85">
+        <v>-6.9</v>
+      </c>
+      <c r="D85">
+        <v>1.8</v>
+      </c>
+      <c r="E85">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Retail trade confidence indicator (5%)</t>
+        </is>
+      </c>
+      <c r="B86" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C86">
+        <v>3.8</v>
+      </c>
+      <c r="D86">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="E86">
+        <v>14.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6765,7 +6993,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8359,6 +8587,63 @@
         <v>42.6</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Services confidence indicator (30 %)</t>
+        </is>
+      </c>
+      <c r="B84" s="2">
+        <v>44501</v>
+      </c>
+      <c r="C84">
+        <v>16.3</v>
+      </c>
+      <c r="D84">
+        <v>20.2</v>
+      </c>
+      <c r="E84">
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Services confidence indicator (30 %)</t>
+        </is>
+      </c>
+      <c r="B85" s="2">
+        <v>44531</v>
+      </c>
+      <c r="C85">
+        <v>5.7</v>
+      </c>
+      <c r="D85">
+        <v>20.9</v>
+      </c>
+      <c r="E85">
+        <v>39.3</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Services confidence indicator (30 %)</t>
+        </is>
+      </c>
+      <c r="B86" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C86">
+        <v>6.9</v>
+      </c>
+      <c r="D86">
+        <v>15.3</v>
+      </c>
+      <c r="E86">
+        <v>31.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8366,7 +8651,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8412,13 +8697,13 @@
         <v>42005</v>
       </c>
       <c r="C2">
-        <v>103.9</v>
+        <v>103.4</v>
       </c>
       <c r="D2">
-        <v>90.40000000000001</v>
+        <v>90.09999999999999</v>
       </c>
       <c r="E2">
-        <v>103.4</v>
+        <v>102.5</v>
       </c>
     </row>
     <row r="3">
@@ -8431,13 +8716,13 @@
         <v>42036</v>
       </c>
       <c r="C3">
-        <v>103.3</v>
+        <v>102.9</v>
       </c>
       <c r="D3">
-        <v>89.2</v>
+        <v>88.90000000000001</v>
       </c>
       <c r="E3">
-        <v>102.1</v>
+        <v>101.3</v>
       </c>
     </row>
     <row r="4">
@@ -8450,13 +8735,13 @@
         <v>42064</v>
       </c>
       <c r="C4">
-        <v>104.6</v>
+        <v>104.1</v>
       </c>
       <c r="D4">
-        <v>91.09999999999999</v>
+        <v>90.8</v>
       </c>
       <c r="E4">
-        <v>100.2</v>
+        <v>99.59999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -8469,13 +8754,13 @@
         <v>42095</v>
       </c>
       <c r="C5">
-        <v>104.6</v>
+        <v>104.1</v>
       </c>
       <c r="D5">
-        <v>91.2</v>
+        <v>91</v>
       </c>
       <c r="E5">
-        <v>98.40000000000001</v>
+        <v>97.90000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -8488,13 +8773,13 @@
         <v>42125</v>
       </c>
       <c r="C6">
-        <v>104.6</v>
+        <v>104.1</v>
       </c>
       <c r="D6">
-        <v>90</v>
+        <v>89.8</v>
       </c>
       <c r="E6">
-        <v>102</v>
+        <v>101.2</v>
       </c>
     </row>
     <row r="7">
@@ -8507,13 +8792,13 @@
         <v>42156</v>
       </c>
       <c r="C7">
-        <v>105.5</v>
+        <v>105</v>
       </c>
       <c r="D7">
-        <v>90.5</v>
+        <v>90.3</v>
       </c>
       <c r="E7">
-        <v>100.8</v>
+        <v>100.2</v>
       </c>
     </row>
     <row r="8">
@@ -8526,13 +8811,13 @@
         <v>42186</v>
       </c>
       <c r="C8">
-        <v>106.1</v>
+        <v>105.6</v>
       </c>
       <c r="D8">
-        <v>92.5</v>
+        <v>92.2</v>
       </c>
       <c r="E8">
-        <v>101.4</v>
+        <v>100.6</v>
       </c>
     </row>
     <row r="9">
@@ -8545,13 +8830,13 @@
         <v>42217</v>
       </c>
       <c r="C9">
-        <v>106.5</v>
+        <v>106.1</v>
       </c>
       <c r="D9">
-        <v>91.09999999999999</v>
+        <v>90.90000000000001</v>
       </c>
       <c r="E9">
-        <v>103.9</v>
+        <v>103.1</v>
       </c>
     </row>
     <row r="10">
@@ -8564,13 +8849,13 @@
         <v>42248</v>
       </c>
       <c r="C10">
-        <v>107.5</v>
+        <v>107</v>
       </c>
       <c r="D10">
-        <v>92.5</v>
+        <v>92.2</v>
       </c>
       <c r="E10">
-        <v>104.7</v>
+        <v>103.6</v>
       </c>
     </row>
     <row r="11">
@@ -8583,13 +8868,13 @@
         <v>42278</v>
       </c>
       <c r="C11">
-        <v>106.9</v>
+        <v>106.4</v>
       </c>
       <c r="D11">
-        <v>94.5</v>
+        <v>94.2</v>
       </c>
       <c r="E11">
-        <v>105.6</v>
+        <v>104.6</v>
       </c>
     </row>
     <row r="12">
@@ -8602,13 +8887,13 @@
         <v>42309</v>
       </c>
       <c r="C12">
-        <v>107</v>
+        <v>106.5</v>
       </c>
       <c r="D12">
-        <v>95.40000000000001</v>
+        <v>95.2</v>
       </c>
       <c r="E12">
-        <v>104.9</v>
+        <v>103.7</v>
       </c>
     </row>
     <row r="13">
@@ -8621,13 +8906,13 @@
         <v>42339</v>
       </c>
       <c r="C13">
-        <v>106.4</v>
+        <v>105.9</v>
       </c>
       <c r="D13">
-        <v>94.09999999999999</v>
+        <v>93.8</v>
       </c>
       <c r="E13">
-        <v>108.2</v>
+        <v>106.9</v>
       </c>
     </row>
     <row r="14">
@@ -8640,13 +8925,13 @@
         <v>42370</v>
       </c>
       <c r="C14">
-        <v>105.3</v>
+        <v>104.9</v>
       </c>
       <c r="D14">
-        <v>96.3</v>
+        <v>96</v>
       </c>
       <c r="E14">
-        <v>109.6</v>
+        <v>107.9</v>
       </c>
     </row>
     <row r="15">
@@ -8659,13 +8944,13 @@
         <v>42401</v>
       </c>
       <c r="C15">
-        <v>104.1</v>
+        <v>103.7</v>
       </c>
       <c r="D15">
-        <v>92.2</v>
+        <v>91.90000000000001</v>
       </c>
       <c r="E15">
-        <v>106.7</v>
+        <v>105.5</v>
       </c>
     </row>
     <row r="16">
@@ -8678,13 +8963,13 @@
         <v>42430</v>
       </c>
       <c r="C16">
-        <v>103.7</v>
+        <v>103.3</v>
       </c>
       <c r="D16">
-        <v>93.3</v>
+        <v>93</v>
       </c>
       <c r="E16">
-        <v>105</v>
+        <v>103.8</v>
       </c>
     </row>
     <row r="17">
@@ -8697,13 +8982,13 @@
         <v>42461</v>
       </c>
       <c r="C17">
-        <v>104.3</v>
+        <v>103.9</v>
       </c>
       <c r="D17">
-        <v>94.09999999999999</v>
+        <v>93.8</v>
       </c>
       <c r="E17">
-        <v>103.2</v>
+        <v>102.1</v>
       </c>
     </row>
     <row r="18">
@@ -8716,13 +9001,13 @@
         <v>42491</v>
       </c>
       <c r="C18">
-        <v>104.3</v>
+        <v>103.8</v>
       </c>
       <c r="D18">
-        <v>93.59999999999999</v>
+        <v>93.3</v>
       </c>
       <c r="E18">
-        <v>102.2</v>
+        <v>101.1</v>
       </c>
     </row>
     <row r="19">
@@ -8735,13 +9020,13 @@
         <v>42522</v>
       </c>
       <c r="C19">
-        <v>105.5</v>
+        <v>105</v>
       </c>
       <c r="D19">
-        <v>95.7</v>
+        <v>95.40000000000001</v>
       </c>
       <c r="E19">
-        <v>102.3</v>
+        <v>101.4</v>
       </c>
     </row>
     <row r="20">
@@ -8754,13 +9039,13 @@
         <v>42552</v>
       </c>
       <c r="C20">
-        <v>105.9</v>
+        <v>105.4</v>
       </c>
       <c r="D20">
-        <v>95.3</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="E20">
-        <v>101.3</v>
+        <v>100.4</v>
       </c>
     </row>
     <row r="21">
@@ -8773,13 +9058,13 @@
         <v>42583</v>
       </c>
       <c r="C21">
-        <v>105.4</v>
+        <v>104.9</v>
       </c>
       <c r="D21">
-        <v>99.59999999999999</v>
+        <v>99.2</v>
       </c>
       <c r="E21">
-        <v>100</v>
+        <v>99.40000000000001</v>
       </c>
     </row>
     <row r="22">
@@ -8792,13 +9077,13 @@
         <v>42614</v>
       </c>
       <c r="C22">
-        <v>106.5</v>
+        <v>106</v>
       </c>
       <c r="D22">
-        <v>104.1</v>
+        <v>103.6</v>
       </c>
       <c r="E22">
-        <v>102.5</v>
+        <v>101.8</v>
       </c>
     </row>
     <row r="23">
@@ -8811,13 +9096,13 @@
         <v>42644</v>
       </c>
       <c r="C23">
-        <v>107.9</v>
+        <v>107.4</v>
       </c>
       <c r="D23">
-        <v>101.8</v>
+        <v>101.4</v>
       </c>
       <c r="E23">
-        <v>105.5</v>
+        <v>104.7</v>
       </c>
     </row>
     <row r="24">
@@ -8830,13 +9115,13 @@
         <v>42675</v>
       </c>
       <c r="C24">
-        <v>107.6</v>
+        <v>107.2</v>
       </c>
       <c r="D24">
-        <v>100</v>
+        <v>99.59999999999999</v>
       </c>
       <c r="E24">
-        <v>108.3</v>
+        <v>107.3</v>
       </c>
     </row>
     <row r="25">
@@ -8849,13 +9134,13 @@
         <v>42705</v>
       </c>
       <c r="C25">
-        <v>108.8</v>
+        <v>108.3</v>
       </c>
       <c r="D25">
-        <v>104.5</v>
+        <v>104</v>
       </c>
       <c r="E25">
-        <v>111.1</v>
+        <v>109.7</v>
       </c>
     </row>
     <row r="26">
@@ -8868,13 +9153,13 @@
         <v>42736</v>
       </c>
       <c r="C26">
-        <v>108.3</v>
+        <v>107.8</v>
       </c>
       <c r="D26">
-        <v>104.9</v>
+        <v>104.4</v>
       </c>
       <c r="E26">
-        <v>109.9</v>
+        <v>108.5</v>
       </c>
     </row>
     <row r="27">
@@ -8887,13 +9172,13 @@
         <v>42767</v>
       </c>
       <c r="C27">
-        <v>107.9</v>
+        <v>107.4</v>
       </c>
       <c r="D27">
-        <v>103.3</v>
+        <v>102.9</v>
       </c>
       <c r="E27">
-        <v>110.5</v>
+        <v>109.1</v>
       </c>
     </row>
     <row r="28">
@@ -8906,13 +9191,13 @@
         <v>42795</v>
       </c>
       <c r="C28">
-        <v>108.3</v>
+        <v>107.7</v>
       </c>
       <c r="D28">
-        <v>105.6</v>
+        <v>105.1</v>
       </c>
       <c r="E28">
-        <v>108</v>
+        <v>106.8</v>
       </c>
     </row>
     <row r="29">
@@ -8925,13 +9210,13 @@
         <v>42826</v>
       </c>
       <c r="C29">
-        <v>109.8</v>
+        <v>109.2</v>
       </c>
       <c r="D29">
-        <v>105.9</v>
+        <v>105.5</v>
       </c>
       <c r="E29">
-        <v>111.7</v>
+        <v>110.1</v>
       </c>
     </row>
     <row r="30">
@@ -8944,13 +9229,13 @@
         <v>42856</v>
       </c>
       <c r="C30">
-        <v>109.2</v>
+        <v>108.6</v>
       </c>
       <c r="D30">
-        <v>107.5</v>
+        <v>107</v>
       </c>
       <c r="E30">
-        <v>111.1</v>
+        <v>109.6</v>
       </c>
     </row>
     <row r="31">
@@ -8963,13 +9248,13 @@
         <v>42887</v>
       </c>
       <c r="C31">
-        <v>110.7</v>
+        <v>110.1</v>
       </c>
       <c r="D31">
-        <v>108.2</v>
+        <v>107.8</v>
       </c>
       <c r="E31">
-        <v>111.1</v>
+        <v>109.5</v>
       </c>
     </row>
     <row r="32">
@@ -8982,13 +9267,13 @@
         <v>42917</v>
       </c>
       <c r="C32">
-        <v>112</v>
+        <v>111.3</v>
       </c>
       <c r="D32">
-        <v>108.8</v>
+        <v>108.2</v>
       </c>
       <c r="E32">
-        <v>110.5</v>
+        <v>108.9</v>
       </c>
     </row>
     <row r="33">
@@ -9001,13 +9286,13 @@
         <v>42948</v>
       </c>
       <c r="C33">
-        <v>111.6</v>
+        <v>111</v>
       </c>
       <c r="D33">
-        <v>109.3</v>
+        <v>108.8</v>
       </c>
       <c r="E33">
-        <v>109</v>
+        <v>107.7</v>
       </c>
     </row>
     <row r="34">
@@ -9020,13 +9305,13 @@
         <v>42979</v>
       </c>
       <c r="C34">
-        <v>112.1</v>
+        <v>111.4</v>
       </c>
       <c r="D34">
-        <v>111.6</v>
+        <v>111</v>
       </c>
       <c r="E34">
-        <v>110.9</v>
+        <v>109.5</v>
       </c>
     </row>
     <row r="35">
@@ -9039,13 +9324,13 @@
         <v>43009</v>
       </c>
       <c r="C35">
-        <v>113.6</v>
+        <v>112.9</v>
       </c>
       <c r="D35">
-        <v>112.3</v>
+        <v>111.8</v>
       </c>
       <c r="E35">
-        <v>112</v>
+        <v>110.5</v>
       </c>
     </row>
     <row r="36">
@@ -9058,13 +9343,13 @@
         <v>43040</v>
       </c>
       <c r="C36">
-        <v>114</v>
+        <v>113.2</v>
       </c>
       <c r="D36">
+        <v>110.4</v>
+      </c>
+      <c r="E36">
         <v>110.9</v>
-      </c>
-      <c r="E36">
-        <v>112.4</v>
       </c>
     </row>
     <row r="37">
@@ -9077,13 +9362,13 @@
         <v>43070</v>
       </c>
       <c r="C37">
-        <v>114.6</v>
+        <v>113.8</v>
       </c>
       <c r="D37">
-        <v>115.8</v>
+        <v>115</v>
       </c>
       <c r="E37">
-        <v>110.1</v>
+        <v>108.8</v>
       </c>
     </row>
     <row r="38">
@@ -9096,13 +9381,13 @@
         <v>43101</v>
       </c>
       <c r="C38">
-        <v>115.1</v>
+        <v>114.4</v>
       </c>
       <c r="D38">
-        <v>112.5</v>
+        <v>111.9</v>
       </c>
       <c r="E38">
-        <v>110.5</v>
+        <v>109.2</v>
       </c>
     </row>
     <row r="39">
@@ -9115,13 +9400,13 @@
         <v>43132</v>
       </c>
       <c r="C39">
-        <v>114.5</v>
+        <v>113.8</v>
       </c>
       <c r="D39">
-        <v>113.7</v>
+        <v>113.1</v>
       </c>
       <c r="E39">
-        <v>110.4</v>
+        <v>108.8</v>
       </c>
     </row>
     <row r="40">
@@ -9134,13 +9419,13 @@
         <v>43160</v>
       </c>
       <c r="C40">
-        <v>112.4</v>
+        <v>111.7</v>
       </c>
       <c r="D40">
-        <v>112.1</v>
+        <v>111.6</v>
       </c>
       <c r="E40">
-        <v>109.6</v>
+        <v>108.2</v>
       </c>
     </row>
     <row r="41">
@@ -9153,13 +9438,13 @@
         <v>43191</v>
       </c>
       <c r="C41">
-        <v>111.8</v>
+        <v>111.2</v>
       </c>
       <c r="D41">
-        <v>110.3</v>
+        <v>109.8</v>
       </c>
       <c r="E41">
-        <v>110.6</v>
+        <v>108.9</v>
       </c>
     </row>
     <row r="42">
@@ -9172,13 +9457,13 @@
         <v>43221</v>
       </c>
       <c r="C42">
-        <v>112</v>
+        <v>111.3</v>
       </c>
       <c r="D42">
-        <v>111.2</v>
+        <v>110.7</v>
       </c>
       <c r="E42">
-        <v>109.9</v>
+        <v>108.2</v>
       </c>
     </row>
     <row r="43">
@@ -9191,13 +9476,13 @@
         <v>43252</v>
       </c>
       <c r="C43">
-        <v>111.5</v>
+        <v>110.8</v>
       </c>
       <c r="D43">
-        <v>109.1</v>
+        <v>108.6</v>
       </c>
       <c r="E43">
-        <v>108.3</v>
+        <v>106.8</v>
       </c>
     </row>
     <row r="44">
@@ -9210,13 +9495,13 @@
         <v>43282</v>
       </c>
       <c r="C44">
-        <v>112.2</v>
+        <v>111.6</v>
       </c>
       <c r="D44">
-        <v>110.8</v>
+        <v>110.3</v>
       </c>
       <c r="E44">
-        <v>108.4</v>
+        <v>106.9</v>
       </c>
     </row>
     <row r="45">
@@ -9229,13 +9514,13 @@
         <v>43313</v>
       </c>
       <c r="C45">
-        <v>112.3</v>
+        <v>111.7</v>
       </c>
       <c r="D45">
-        <v>110.7</v>
+        <v>110.1</v>
       </c>
       <c r="E45">
-        <v>111.3</v>
+        <v>109.6</v>
       </c>
     </row>
     <row r="46">
@@ -9248,13 +9533,13 @@
         <v>43344</v>
       </c>
       <c r="C46">
-        <v>112.1</v>
+        <v>111.5</v>
       </c>
       <c r="D46">
-        <v>110.5</v>
+        <v>110</v>
       </c>
       <c r="E46">
-        <v>109.8</v>
+        <v>108.4</v>
       </c>
     </row>
     <row r="47">
@@ -9267,13 +9552,13 @@
         <v>43374</v>
       </c>
       <c r="C47">
-        <v>110.8</v>
+        <v>110.3</v>
       </c>
       <c r="D47">
-        <v>105.6</v>
+        <v>105.1</v>
       </c>
       <c r="E47">
-        <v>107.3</v>
+        <v>106.1</v>
       </c>
     </row>
     <row r="48">
@@ -9286,13 +9571,13 @@
         <v>43405</v>
       </c>
       <c r="C48">
-        <v>111.2</v>
+        <v>110.8</v>
       </c>
       <c r="D48">
-        <v>104.9</v>
+        <v>104.4</v>
       </c>
       <c r="E48">
-        <v>106.3</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49">
@@ -9305,13 +9590,13 @@
         <v>43435</v>
       </c>
       <c r="C49">
-        <v>109.2</v>
+        <v>108.7</v>
       </c>
       <c r="D49">
-        <v>101.7</v>
+        <v>101.4</v>
       </c>
       <c r="E49">
-        <v>107.2</v>
+        <v>105.8</v>
       </c>
     </row>
     <row r="50">
@@ -9324,13 +9609,13 @@
         <v>43466</v>
       </c>
       <c r="C50">
-        <v>108.3</v>
+        <v>107.8</v>
       </c>
       <c r="D50">
-        <v>102.5</v>
+        <v>102.1</v>
       </c>
       <c r="E50">
-        <v>103.1</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51">
@@ -9343,13 +9628,13 @@
         <v>43497</v>
       </c>
       <c r="C51">
-        <v>108.1</v>
+        <v>107.8</v>
       </c>
       <c r="D51">
-        <v>101.1</v>
+        <v>100.7</v>
       </c>
       <c r="E51">
-        <v>103.9</v>
+        <v>102.6</v>
       </c>
     </row>
     <row r="52">
@@ -9362,13 +9647,13 @@
         <v>43525</v>
       </c>
       <c r="C52">
-        <v>106.3</v>
+        <v>106</v>
       </c>
       <c r="D52">
-        <v>99.3</v>
+        <v>99</v>
       </c>
       <c r="E52">
-        <v>102.9</v>
+        <v>101.7</v>
       </c>
     </row>
     <row r="53">
@@ -9381,13 +9666,13 @@
         <v>43556</v>
       </c>
       <c r="C53">
-        <v>104.9</v>
+        <v>104.7</v>
       </c>
       <c r="D53">
-        <v>99</v>
+        <v>98.59999999999999</v>
       </c>
       <c r="E53">
-        <v>105.6</v>
+        <v>104.3</v>
       </c>
     </row>
     <row r="54">
@@ -9400,13 +9685,13 @@
         <v>43586</v>
       </c>
       <c r="C54">
-        <v>105.3</v>
+        <v>105</v>
       </c>
       <c r="D54">
-        <v>100.8</v>
+        <v>100.4</v>
       </c>
       <c r="E54">
-        <v>100.2</v>
+        <v>99.09999999999999</v>
       </c>
     </row>
     <row r="55">
@@ -9419,13 +9704,13 @@
         <v>43617</v>
       </c>
       <c r="C55">
-        <v>102.4</v>
+        <v>102.2</v>
       </c>
       <c r="D55">
-        <v>98.90000000000001</v>
+        <v>98.59999999999999</v>
       </c>
       <c r="E55">
-        <v>100.1</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="56">
@@ -9438,13 +9723,13 @@
         <v>43647</v>
       </c>
       <c r="C56">
-        <v>99.7</v>
+        <v>99.59999999999999</v>
       </c>
       <c r="D56">
-        <v>97.8</v>
+        <v>97.5</v>
       </c>
       <c r="E56">
-        <v>99.2</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="57">
@@ -9457,13 +9742,13 @@
         <v>43678</v>
       </c>
       <c r="C57">
-        <v>100.1</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="D57">
-        <v>99.09999999999999</v>
+        <v>98.7</v>
       </c>
       <c r="E57">
-        <v>97.5</v>
+        <v>96.7</v>
       </c>
     </row>
     <row r="58">
@@ -9476,13 +9761,13 @@
         <v>43709</v>
       </c>
       <c r="C58">
-        <v>98.90000000000001</v>
+        <v>98.8</v>
       </c>
       <c r="D58">
-        <v>99</v>
+        <v>98.59999999999999</v>
       </c>
       <c r="E58">
-        <v>95.5</v>
+        <v>94.59999999999999</v>
       </c>
     </row>
     <row r="59">
@@ -9495,13 +9780,13 @@
         <v>43739</v>
       </c>
       <c r="C59">
-        <v>98.7</v>
+        <v>98.59999999999999</v>
       </c>
       <c r="D59">
-        <v>95.40000000000001</v>
+        <v>95</v>
       </c>
       <c r="E59">
-        <v>96.59999999999999</v>
+        <v>95.90000000000001</v>
       </c>
     </row>
     <row r="60">
@@ -9514,13 +9799,13 @@
         <v>43770</v>
       </c>
       <c r="C60">
-        <v>99.09999999999999</v>
+        <v>99</v>
       </c>
       <c r="D60">
-        <v>97.2</v>
+        <v>96.90000000000001</v>
       </c>
       <c r="E60">
-        <v>95.8</v>
+        <v>95.09999999999999</v>
       </c>
     </row>
     <row r="61">
@@ -9533,13 +9818,13 @@
         <v>43800</v>
       </c>
       <c r="C61">
-        <v>99.59999999999999</v>
+        <v>99.5</v>
       </c>
       <c r="D61">
-        <v>97</v>
+        <v>96.59999999999999</v>
       </c>
       <c r="E61">
-        <v>95.40000000000001</v>
+        <v>94.8</v>
       </c>
     </row>
     <row r="62">
@@ -9552,13 +9837,13 @@
         <v>43831</v>
       </c>
       <c r="C62">
-        <v>101.6</v>
+        <v>101.4</v>
       </c>
       <c r="D62">
-        <v>95.5</v>
+        <v>95.2</v>
       </c>
       <c r="E62">
-        <v>97.40000000000001</v>
+        <v>96.59999999999999</v>
       </c>
     </row>
     <row r="63">
@@ -9571,13 +9856,13 @@
         <v>43862</v>
       </c>
       <c r="C63">
-        <v>102.2</v>
+        <v>101.9</v>
       </c>
       <c r="D63">
-        <v>94.5</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="E63">
-        <v>99.7</v>
+        <v>98.7</v>
       </c>
     </row>
     <row r="64">
@@ -9590,13 +9875,13 @@
         <v>43891</v>
       </c>
       <c r="C64">
-        <v>92.7</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="D64">
-        <v>91.8</v>
+        <v>91.40000000000001</v>
       </c>
       <c r="E64">
-        <v>94.59999999999999</v>
+        <v>93.59999999999999</v>
       </c>
     </row>
     <row r="65">
@@ -9609,10 +9894,10 @@
         <v>43922</v>
       </c>
       <c r="C65">
-        <v>73.3</v>
+        <v>73.2</v>
       </c>
       <c r="D65">
-        <v>71.2</v>
+        <v>71.09999999999999</v>
       </c>
       <c r="E65">
         <v>69.90000000000001</v>
@@ -9628,10 +9913,10 @@
         <v>43952</v>
       </c>
       <c r="C66">
-        <v>76.5</v>
+        <v>76.40000000000001</v>
       </c>
       <c r="D66">
-        <v>75.09999999999999</v>
+        <v>74.8</v>
       </c>
       <c r="E66">
         <v>71.59999999999999</v>
@@ -9647,13 +9932,13 @@
         <v>43983</v>
       </c>
       <c r="C67">
-        <v>82.90000000000001</v>
+        <v>82.7</v>
       </c>
       <c r="D67">
-        <v>78.59999999999999</v>
+        <v>78.3</v>
       </c>
       <c r="E67">
-        <v>80</v>
+        <v>79.7</v>
       </c>
     </row>
     <row r="68">
@@ -9666,13 +9951,13 @@
         <v>44013</v>
       </c>
       <c r="C68">
-        <v>89.09999999999999</v>
+        <v>88.8</v>
       </c>
       <c r="D68">
-        <v>87.7</v>
+        <v>87.3</v>
       </c>
       <c r="E68">
-        <v>87.2</v>
+        <v>86.59999999999999</v>
       </c>
     </row>
     <row r="69">
@@ -9685,13 +9970,13 @@
         <v>44044</v>
       </c>
       <c r="C69">
-        <v>94.90000000000001</v>
+        <v>94.5</v>
       </c>
       <c r="D69">
-        <v>85.40000000000001</v>
+        <v>85.09999999999999</v>
       </c>
       <c r="E69">
-        <v>90.09999999999999</v>
+        <v>89.3</v>
       </c>
     </row>
     <row r="70">
@@ -9704,13 +9989,13 @@
         <v>44075</v>
       </c>
       <c r="C70">
-        <v>96.09999999999999</v>
+        <v>95.59999999999999</v>
       </c>
       <c r="D70">
-        <v>84</v>
+        <v>83.7</v>
       </c>
       <c r="E70">
-        <v>95.3</v>
+        <v>94.3</v>
       </c>
     </row>
     <row r="71">
@@ -9723,13 +10008,13 @@
         <v>44105</v>
       </c>
       <c r="C71">
-        <v>97.59999999999999</v>
+        <v>96.90000000000001</v>
       </c>
       <c r="D71">
-        <v>86.8</v>
+        <v>86.40000000000001</v>
       </c>
       <c r="E71">
-        <v>96.3</v>
+        <v>95.3</v>
       </c>
     </row>
     <row r="72">
@@ -9742,13 +10027,13 @@
         <v>44136</v>
       </c>
       <c r="C72">
-        <v>94.90000000000001</v>
+        <v>94.2</v>
       </c>
       <c r="D72">
-        <v>88.2</v>
+        <v>87.8</v>
       </c>
       <c r="E72">
-        <v>97.09999999999999</v>
+        <v>95.90000000000001</v>
       </c>
     </row>
     <row r="73">
@@ -9761,13 +10046,13 @@
         <v>44166</v>
       </c>
       <c r="C73">
-        <v>95.09999999999999</v>
+        <v>94.3</v>
       </c>
       <c r="D73">
-        <v>90.7</v>
+        <v>90.3</v>
       </c>
       <c r="E73">
-        <v>96.8</v>
+        <v>95.7</v>
       </c>
     </row>
     <row r="74">
@@ -9780,13 +10065,13 @@
         <v>44197</v>
       </c>
       <c r="C74">
-        <v>92.8</v>
+        <v>92</v>
       </c>
       <c r="D74">
-        <v>95.59999999999999</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="E74">
-        <v>101.8</v>
+        <v>100.4</v>
       </c>
     </row>
     <row r="75">
@@ -9799,13 +10084,13 @@
         <v>44228</v>
       </c>
       <c r="C75">
-        <v>95.8</v>
+        <v>94.90000000000001</v>
       </c>
       <c r="D75">
-        <v>93.59999999999999</v>
+        <v>93.2</v>
       </c>
       <c r="E75">
-        <v>104.9</v>
+        <v>103.4</v>
       </c>
     </row>
     <row r="76">
@@ -9818,13 +10103,13 @@
         <v>44256</v>
       </c>
       <c r="C76">
-        <v>103.7</v>
+        <v>102.8</v>
       </c>
       <c r="D76">
-        <v>96.59999999999999</v>
+        <v>96</v>
       </c>
       <c r="E76">
-        <v>106.7</v>
+        <v>105</v>
       </c>
     </row>
     <row r="77">
@@ -9837,13 +10122,13 @@
         <v>44287</v>
       </c>
       <c r="C77">
-        <v>109.4</v>
+        <v>108.2</v>
       </c>
       <c r="D77">
-        <v>109.8</v>
+        <v>109</v>
       </c>
       <c r="E77">
-        <v>117.5</v>
+        <v>115.3</v>
       </c>
     </row>
     <row r="78">
@@ -9856,13 +10141,13 @@
         <v>44317</v>
       </c>
       <c r="C78">
-        <v>112.2</v>
+        <v>111</v>
       </c>
       <c r="D78">
-        <v>110.4</v>
+        <v>109.8</v>
       </c>
       <c r="E78">
-        <v>122.6</v>
+        <v>120.2</v>
       </c>
     </row>
     <row r="79">
@@ -9875,13 +10160,13 @@
         <v>44348</v>
       </c>
       <c r="C79">
-        <v>117.2</v>
+        <v>116</v>
       </c>
       <c r="D79">
-        <v>114.8</v>
+        <v>114</v>
       </c>
       <c r="E79">
-        <v>120.8</v>
+        <v>118.5</v>
       </c>
     </row>
     <row r="80">
@@ -9894,13 +10179,13 @@
         <v>44378</v>
       </c>
       <c r="C80">
-        <v>117.5</v>
+        <v>116.2</v>
       </c>
       <c r="D80">
-        <v>113.9</v>
+        <v>113.1</v>
       </c>
       <c r="E80">
-        <v>123.6</v>
+        <v>120.8</v>
       </c>
     </row>
     <row r="81">
@@ -9913,13 +10198,13 @@
         <v>44409</v>
       </c>
       <c r="C81">
-        <v>117.2</v>
+        <v>115.8</v>
       </c>
       <c r="D81">
-        <v>116.1</v>
+        <v>115.3</v>
       </c>
       <c r="E81">
-        <v>123.2</v>
+        <v>120.5</v>
       </c>
     </row>
     <row r="82">
@@ -9932,13 +10217,13 @@
         <v>44440</v>
       </c>
       <c r="C82">
-        <v>118</v>
+        <v>116.6</v>
       </c>
       <c r="D82">
-        <v>116.8</v>
+        <v>115.9</v>
       </c>
       <c r="E82">
-        <v>121.7</v>
+        <v>118.9</v>
       </c>
     </row>
     <row r="83">
@@ -9951,13 +10236,70 @@
         <v>44470</v>
       </c>
       <c r="C83">
-        <v>117.5</v>
+        <v>116</v>
       </c>
       <c r="D83">
-        <v>117</v>
+        <v>116.2</v>
       </c>
       <c r="E83">
-        <v>123.8</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>The Economic sentiment indicator is a composite measure (average = 100)</t>
+        </is>
+      </c>
+      <c r="B84" s="2">
+        <v>44501</v>
+      </c>
+      <c r="C84">
+        <v>114.3</v>
+      </c>
+      <c r="D84">
+        <v>116.8</v>
+      </c>
+      <c r="E84">
+        <v>119.1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>The Economic sentiment indicator is a composite measure (average = 100)</t>
+        </is>
+      </c>
+      <c r="B85" s="2">
+        <v>44531</v>
+      </c>
+      <c r="C85">
+        <v>111.5</v>
+      </c>
+      <c r="D85">
+        <v>111</v>
+      </c>
+      <c r="E85">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>The Economic sentiment indicator is a composite measure (average = 100)</t>
+        </is>
+      </c>
+      <c r="B86" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C86">
+        <v>112.3</v>
+      </c>
+      <c r="D86">
+        <v>110.7</v>
+      </c>
+      <c r="E86">
+        <v>112.7</v>
       </c>
     </row>
   </sheetData>
@@ -9967,7 +10309,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10013,13 +10355,13 @@
         <v>42005</v>
       </c>
       <c r="C2">
-        <v>103.2</v>
+        <v>102.8</v>
       </c>
       <c r="D2">
-        <v>90.5</v>
+        <v>90.2</v>
       </c>
       <c r="E2">
-        <v>106.1</v>
+        <v>105.4</v>
       </c>
     </row>
     <row r="3">
@@ -10032,13 +10374,13 @@
         <v>42036</v>
       </c>
       <c r="C3">
-        <v>103.3</v>
+        <v>102.9</v>
       </c>
       <c r="D3">
-        <v>91.3</v>
+        <v>90.90000000000001</v>
       </c>
       <c r="E3">
-        <v>105.8</v>
+        <v>105.1</v>
       </c>
     </row>
     <row r="4">
@@ -10051,13 +10393,13 @@
         <v>42064</v>
       </c>
       <c r="C4">
-        <v>104.1</v>
+        <v>103.8</v>
       </c>
       <c r="D4">
-        <v>91.2</v>
+        <v>90.90000000000001</v>
       </c>
       <c r="E4">
-        <v>105.7</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5">
@@ -10070,13 +10412,13 @@
         <v>42095</v>
       </c>
       <c r="C5">
-        <v>104.9</v>
+        <v>104.5</v>
       </c>
       <c r="D5">
-        <v>87.3</v>
+        <v>87</v>
       </c>
       <c r="E5">
-        <v>104.3</v>
+        <v>103.7</v>
       </c>
     </row>
     <row r="6">
@@ -10089,13 +10431,13 @@
         <v>42125</v>
       </c>
       <c r="C6">
-        <v>105.3</v>
+        <v>104.9</v>
       </c>
       <c r="D6">
-        <v>90.3</v>
+        <v>89.90000000000001</v>
       </c>
       <c r="E6">
-        <v>103.4</v>
+        <v>102.7</v>
       </c>
     </row>
     <row r="7">
@@ -10108,13 +10450,13 @@
         <v>42156</v>
       </c>
       <c r="C7">
-        <v>106.7</v>
+        <v>106.3</v>
       </c>
       <c r="D7">
-        <v>88.7</v>
+        <v>88.5</v>
       </c>
       <c r="E7">
-        <v>103.1</v>
+        <v>102.5</v>
       </c>
     </row>
     <row r="8">
@@ -10127,13 +10469,13 @@
         <v>42186</v>
       </c>
       <c r="C8">
-        <v>106.7</v>
+        <v>106.3</v>
       </c>
       <c r="D8">
-        <v>90.3</v>
+        <v>90.09999999999999</v>
       </c>
       <c r="E8">
-        <v>103.8</v>
+        <v>103.2</v>
       </c>
     </row>
     <row r="9">
@@ -10146,13 +10488,13 @@
         <v>42217</v>
       </c>
       <c r="C9">
-        <v>106.6</v>
+        <v>106.2</v>
       </c>
       <c r="D9">
-        <v>89.59999999999999</v>
+        <v>89.5</v>
       </c>
       <c r="E9">
-        <v>103.3</v>
+        <v>102.7</v>
       </c>
     </row>
     <row r="10">
@@ -10165,13 +10507,13 @@
         <v>42248</v>
       </c>
       <c r="C10">
-        <v>106.6</v>
+        <v>106.3</v>
       </c>
       <c r="D10">
-        <v>87.8</v>
+        <v>87.59999999999999</v>
       </c>
       <c r="E10">
-        <v>105.3</v>
+        <v>104.7</v>
       </c>
     </row>
     <row r="11">
@@ -10184,13 +10526,13 @@
         <v>42278</v>
       </c>
       <c r="C11">
-        <v>108.2</v>
+        <v>107.8</v>
       </c>
       <c r="D11">
-        <v>87.3</v>
+        <v>87</v>
       </c>
       <c r="E11">
-        <v>106.6</v>
+        <v>105.9</v>
       </c>
     </row>
     <row r="12">
@@ -10203,13 +10545,13 @@
         <v>42309</v>
       </c>
       <c r="C12">
-        <v>109.1</v>
+        <v>108.7</v>
       </c>
       <c r="D12">
-        <v>93.3</v>
+        <v>93</v>
       </c>
       <c r="E12">
-        <v>106.4</v>
+        <v>105.8</v>
       </c>
     </row>
     <row r="13">
@@ -10222,13 +10564,13 @@
         <v>42339</v>
       </c>
       <c r="C13">
-        <v>109.3</v>
+        <v>109</v>
       </c>
       <c r="D13">
-        <v>96.09999999999999</v>
+        <v>95.7</v>
       </c>
       <c r="E13">
-        <v>105.6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14">
@@ -10241,13 +10583,13 @@
         <v>42370</v>
       </c>
       <c r="C14">
-        <v>109.4</v>
+        <v>109</v>
       </c>
       <c r="D14">
-        <v>94.09999999999999</v>
+        <v>93.8</v>
       </c>
       <c r="E14">
-        <v>106.1</v>
+        <v>105.4</v>
       </c>
     </row>
     <row r="15">
@@ -10260,13 +10602,13 @@
         <v>42401</v>
       </c>
       <c r="C15">
-        <v>106.2</v>
+        <v>105.8</v>
       </c>
       <c r="D15">
-        <v>92.3</v>
+        <v>92</v>
       </c>
       <c r="E15">
-        <v>105.7</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16">
@@ -10279,13 +10621,13 @@
         <v>42430</v>
       </c>
       <c r="C16">
-        <v>104.5</v>
+        <v>104.2</v>
       </c>
       <c r="D16">
-        <v>94.09999999999999</v>
+        <v>93.90000000000001</v>
       </c>
       <c r="E16">
-        <v>106.1</v>
+        <v>105.4</v>
       </c>
     </row>
     <row r="17">
@@ -10298,13 +10640,13 @@
         <v>42461</v>
       </c>
       <c r="C17">
-        <v>106.4</v>
+        <v>106.1</v>
       </c>
       <c r="D17">
-        <v>96.90000000000001</v>
+        <v>96.5</v>
       </c>
       <c r="E17">
-        <v>103.9</v>
+        <v>103.4</v>
       </c>
     </row>
     <row r="18">
@@ -10317,13 +10659,13 @@
         <v>42491</v>
       </c>
       <c r="C18">
-        <v>106.2</v>
+        <v>105.9</v>
       </c>
       <c r="D18">
-        <v>93.5</v>
+        <v>93.3</v>
       </c>
       <c r="E18">
-        <v>103.6</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19">
@@ -10336,13 +10678,13 @@
         <v>42522</v>
       </c>
       <c r="C19">
-        <v>106.6</v>
+        <v>106.3</v>
       </c>
       <c r="D19">
-        <v>95.5</v>
+        <v>95.2</v>
       </c>
       <c r="E19">
-        <v>105.7</v>
+        <v>105.1</v>
       </c>
     </row>
     <row r="20">
@@ -10355,13 +10697,13 @@
         <v>42552</v>
       </c>
       <c r="C20">
-        <v>107.8</v>
+        <v>107.4</v>
       </c>
       <c r="D20">
-        <v>97</v>
+        <v>96.7</v>
       </c>
       <c r="E20">
-        <v>104.5</v>
+        <v>103.9</v>
       </c>
     </row>
     <row r="21">
@@ -10374,13 +10716,13 @@
         <v>42583</v>
       </c>
       <c r="C21">
-        <v>108</v>
+        <v>107.7</v>
       </c>
       <c r="D21">
-        <v>95.2</v>
+        <v>94.90000000000001</v>
       </c>
       <c r="E21">
-        <v>106.9</v>
+        <v>106.2</v>
       </c>
     </row>
     <row r="22">
@@ -10393,13 +10735,13 @@
         <v>42614</v>
       </c>
       <c r="C22">
-        <v>109.6</v>
+        <v>109.3</v>
       </c>
       <c r="D22">
-        <v>98.90000000000001</v>
+        <v>98.5</v>
       </c>
       <c r="E22">
-        <v>106.7</v>
+        <v>106.1</v>
       </c>
     </row>
     <row r="23">
@@ -10412,13 +10754,13 @@
         <v>42644</v>
       </c>
       <c r="C23">
-        <v>110.6</v>
+        <v>110.3</v>
       </c>
       <c r="D23">
-        <v>99.5</v>
+        <v>99.09999999999999</v>
       </c>
       <c r="E23">
-        <v>107.9</v>
+        <v>107.3</v>
       </c>
     </row>
     <row r="24">
@@ -10431,13 +10773,13 @@
         <v>42675</v>
       </c>
       <c r="C24">
-        <v>111.1</v>
+        <v>110.7</v>
       </c>
       <c r="D24">
-        <v>99.40000000000001</v>
+        <v>98.90000000000001</v>
       </c>
       <c r="E24">
-        <v>107.6</v>
+        <v>106.9</v>
       </c>
     </row>
     <row r="25">
@@ -10450,13 +10792,13 @@
         <v>42705</v>
       </c>
       <c r="C25">
-        <v>110.9</v>
+        <v>110.5</v>
       </c>
       <c r="D25">
-        <v>99.40000000000001</v>
+        <v>98.90000000000001</v>
       </c>
       <c r="E25">
-        <v>109.2</v>
+        <v>108.5</v>
       </c>
     </row>
     <row r="26">
@@ -10469,13 +10811,13 @@
         <v>42736</v>
       </c>
       <c r="C26">
-        <v>110.2</v>
+        <v>109.9</v>
       </c>
       <c r="D26">
-        <v>100.9</v>
+        <v>100.4</v>
       </c>
       <c r="E26">
-        <v>109.8</v>
+        <v>109.1</v>
       </c>
     </row>
     <row r="27">
@@ -10488,13 +10830,13 @@
         <v>42767</v>
       </c>
       <c r="C27">
-        <v>110.4</v>
+        <v>110</v>
       </c>
       <c r="D27">
-        <v>100.7</v>
+        <v>100.2</v>
       </c>
       <c r="E27">
-        <v>109.4</v>
+        <v>108.8</v>
       </c>
     </row>
     <row r="28">
@@ -10507,13 +10849,13 @@
         <v>42795</v>
       </c>
       <c r="C28">
-        <v>108.8</v>
+        <v>108.4</v>
       </c>
       <c r="D28">
-        <v>99.5</v>
+        <v>99</v>
       </c>
       <c r="E28">
-        <v>109.9</v>
+        <v>109.2</v>
       </c>
     </row>
     <row r="29">
@@ -10526,13 +10868,13 @@
         <v>42826</v>
       </c>
       <c r="C29">
-        <v>111.6</v>
+        <v>111.2</v>
       </c>
       <c r="D29">
-        <v>104.6</v>
+        <v>104</v>
       </c>
       <c r="E29">
-        <v>109</v>
+        <v>108.3</v>
       </c>
     </row>
     <row r="30">
@@ -10545,13 +10887,13 @@
         <v>42856</v>
       </c>
       <c r="C30">
-        <v>110.8</v>
+        <v>110.5</v>
       </c>
       <c r="D30">
-        <v>104.5</v>
+        <v>103.9</v>
       </c>
       <c r="E30">
-        <v>110.5</v>
+        <v>109.7</v>
       </c>
     </row>
     <row r="31">
@@ -10564,13 +10906,13 @@
         <v>42887</v>
       </c>
       <c r="C31">
-        <v>112.9</v>
+        <v>112.6</v>
       </c>
       <c r="D31">
-        <v>101</v>
+        <v>100.4</v>
       </c>
       <c r="E31">
-        <v>111</v>
+        <v>110.2</v>
       </c>
     </row>
     <row r="32">
@@ -10583,13 +10925,13 @@
         <v>42917</v>
       </c>
       <c r="C32">
-        <v>113.7</v>
+        <v>113.4</v>
       </c>
       <c r="D32">
-        <v>101.8</v>
+        <v>101.2</v>
       </c>
       <c r="E32">
-        <v>113.1</v>
+        <v>112.3</v>
       </c>
     </row>
     <row r="33">
@@ -10602,13 +10944,13 @@
         <v>42948</v>
       </c>
       <c r="C33">
-        <v>112.1</v>
+        <v>111.7</v>
       </c>
       <c r="D33">
-        <v>105.8</v>
+        <v>105.1</v>
       </c>
       <c r="E33">
-        <v>111.4</v>
+        <v>110.6</v>
       </c>
     </row>
     <row r="34">
@@ -10621,13 +10963,13 @@
         <v>42979</v>
       </c>
       <c r="C34">
-        <v>112.9</v>
+        <v>112.6</v>
       </c>
       <c r="D34">
-        <v>109.7</v>
+        <v>109</v>
       </c>
       <c r="E34">
-        <v>111.4</v>
+        <v>110.6</v>
       </c>
     </row>
     <row r="35">
@@ -10640,13 +10982,13 @@
         <v>43009</v>
       </c>
       <c r="C35">
-        <v>113.5</v>
+        <v>113.1</v>
       </c>
       <c r="D35">
-        <v>109.5</v>
+        <v>108.8</v>
       </c>
       <c r="E35">
-        <v>113.1</v>
+        <v>112.2</v>
       </c>
     </row>
     <row r="36">
@@ -10659,13 +11001,13 @@
         <v>43040</v>
       </c>
       <c r="C36">
-        <v>113.3</v>
+        <v>112.9</v>
       </c>
       <c r="D36">
-        <v>110.9</v>
+        <v>110.1</v>
       </c>
       <c r="E36">
-        <v>112</v>
+        <v>111.1</v>
       </c>
     </row>
     <row r="37">
@@ -10678,13 +11020,13 @@
         <v>43070</v>
       </c>
       <c r="C37">
-        <v>115.2</v>
+        <v>114.8</v>
       </c>
       <c r="D37">
-        <v>115.3</v>
+        <v>114.5</v>
       </c>
       <c r="E37">
-        <v>111</v>
+        <v>110.1</v>
       </c>
     </row>
     <row r="38">
@@ -10697,13 +11039,13 @@
         <v>43101</v>
       </c>
       <c r="C38">
-        <v>117.1</v>
+        <v>116.7</v>
       </c>
       <c r="D38">
-        <v>113.1</v>
+        <v>112.2</v>
       </c>
       <c r="E38">
-        <v>110.7</v>
+        <v>109.9</v>
       </c>
     </row>
     <row r="39">
@@ -10716,13 +11058,13 @@
         <v>43132</v>
       </c>
       <c r="C39">
-        <v>116.7</v>
+        <v>116.3</v>
       </c>
       <c r="D39">
-        <v>115.9</v>
+        <v>115</v>
       </c>
       <c r="E39">
-        <v>108.1</v>
+        <v>107.3</v>
       </c>
     </row>
     <row r="40">
@@ -10735,13 +11077,13 @@
         <v>43160</v>
       </c>
       <c r="C40">
-        <v>115.2</v>
+        <v>114.8</v>
       </c>
       <c r="D40">
-        <v>114.7</v>
+        <v>113.9</v>
       </c>
       <c r="E40">
-        <v>107.6</v>
+        <v>106.8</v>
       </c>
     </row>
     <row r="41">
@@ -10754,13 +11096,13 @@
         <v>43191</v>
       </c>
       <c r="C41">
-        <v>113.7</v>
+        <v>113.3</v>
       </c>
       <c r="D41">
-        <v>114.2</v>
+        <v>113.4</v>
       </c>
       <c r="E41">
-        <v>108.2</v>
+        <v>107.5</v>
       </c>
     </row>
     <row r="42">
@@ -10773,13 +11115,13 @@
         <v>43221</v>
       </c>
       <c r="C42">
-        <v>115.6</v>
+        <v>115.2</v>
       </c>
       <c r="D42">
-        <v>113.9</v>
+        <v>113.1</v>
       </c>
       <c r="E42">
-        <v>107.4</v>
+        <v>106.8</v>
       </c>
     </row>
     <row r="43">
@@ -10792,13 +11134,13 @@
         <v>43252</v>
       </c>
       <c r="C43">
-        <v>115.5</v>
+        <v>115.1</v>
       </c>
       <c r="D43">
-        <v>112.4</v>
+        <v>111.5</v>
       </c>
       <c r="E43">
-        <v>107</v>
+        <v>106.2</v>
       </c>
     </row>
     <row r="44">
@@ -10811,13 +11153,13 @@
         <v>43282</v>
       </c>
       <c r="C44">
-        <v>115.5</v>
+        <v>115.1</v>
       </c>
       <c r="D44">
-        <v>110.4</v>
+        <v>109.6</v>
       </c>
       <c r="E44">
-        <v>108.1</v>
+        <v>107.3</v>
       </c>
     </row>
     <row r="45">
@@ -10830,13 +11172,13 @@
         <v>43313</v>
       </c>
       <c r="C45">
-        <v>116.9</v>
+        <v>116.5</v>
       </c>
       <c r="D45">
-        <v>112.3</v>
+        <v>111.6</v>
       </c>
       <c r="E45">
-        <v>107.9</v>
+        <v>107.1</v>
       </c>
     </row>
     <row r="46">
@@ -10849,13 +11191,13 @@
         <v>43344</v>
       </c>
       <c r="C46">
-        <v>116.2</v>
+        <v>115.8</v>
       </c>
       <c r="D46">
-        <v>113.5</v>
+        <v>112.7</v>
       </c>
       <c r="E46">
-        <v>109.2</v>
+        <v>108.4</v>
       </c>
     </row>
     <row r="47">
@@ -10868,13 +11210,13 @@
         <v>43374</v>
       </c>
       <c r="C47">
-        <v>115.8</v>
+        <v>115.4</v>
       </c>
       <c r="D47">
-        <v>112.5</v>
+        <v>111.7</v>
       </c>
       <c r="E47">
-        <v>107.2</v>
+        <v>106.4</v>
       </c>
     </row>
     <row r="48">
@@ -10887,13 +11229,13 @@
         <v>43405</v>
       </c>
       <c r="C48">
-        <v>113.8</v>
+        <v>113.4</v>
       </c>
       <c r="D48">
-        <v>110.9</v>
+        <v>110.2</v>
       </c>
       <c r="E48">
-        <v>106.8</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49">
@@ -10906,13 +11248,13 @@
         <v>43435</v>
       </c>
       <c r="C49">
-        <v>114</v>
+        <v>113.7</v>
       </c>
       <c r="D49">
-        <v>109.6</v>
+        <v>108.9</v>
       </c>
       <c r="E49">
-        <v>104.5</v>
+        <v>103.8</v>
       </c>
     </row>
     <row r="50">
@@ -10925,13 +11267,13 @@
         <v>43466</v>
       </c>
       <c r="C50">
-        <v>111.9</v>
+        <v>111.5</v>
       </c>
       <c r="D50">
-        <v>109.4</v>
+        <v>108.8</v>
       </c>
       <c r="E50">
-        <v>106.3</v>
+        <v>105.6</v>
       </c>
     </row>
     <row r="51">
@@ -10944,13 +11286,13 @@
         <v>43497</v>
       </c>
       <c r="C51">
-        <v>112.3</v>
+        <v>112</v>
       </c>
       <c r="D51">
-        <v>109.9</v>
+        <v>109.2</v>
       </c>
       <c r="E51">
-        <v>105.6</v>
+        <v>104.9</v>
       </c>
     </row>
     <row r="52">
@@ -10963,13 +11305,13 @@
         <v>43525</v>
       </c>
       <c r="C52">
-        <v>110.6</v>
+        <v>110.3</v>
       </c>
       <c r="D52">
-        <v>109.9</v>
+        <v>109.1</v>
       </c>
       <c r="E52">
-        <v>105.3</v>
+        <v>104.6</v>
       </c>
     </row>
     <row r="53">
@@ -10982,13 +11324,13 @@
         <v>43556</v>
       </c>
       <c r="C53">
-        <v>110</v>
+        <v>109.7</v>
       </c>
       <c r="D53">
-        <v>107.5</v>
+        <v>106.9</v>
       </c>
       <c r="E53">
-        <v>102.4</v>
+        <v>101.8</v>
       </c>
     </row>
     <row r="54">
@@ -11001,13 +11343,13 @@
         <v>43586</v>
       </c>
       <c r="C54">
-        <v>107.9</v>
+        <v>107.6</v>
       </c>
       <c r="D54">
-        <v>107.2</v>
+        <v>106.7</v>
       </c>
       <c r="E54">
-        <v>103.6</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55">
@@ -11020,13 +11362,13 @@
         <v>43617</v>
       </c>
       <c r="C55">
-        <v>107.4</v>
+        <v>107.1</v>
       </c>
       <c r="D55">
-        <v>109.7</v>
+        <v>109</v>
       </c>
       <c r="E55">
-        <v>102.1</v>
+        <v>101.6</v>
       </c>
     </row>
     <row r="56">
@@ -11039,13 +11381,13 @@
         <v>43647</v>
       </c>
       <c r="C56">
-        <v>106.4</v>
+        <v>106.1</v>
       </c>
       <c r="D56">
-        <v>110.6</v>
+        <v>109.9</v>
       </c>
       <c r="E56">
-        <v>102.2</v>
+        <v>101.7</v>
       </c>
     </row>
     <row r="57">
@@ -11058,13 +11400,13 @@
         <v>43678</v>
       </c>
       <c r="C57">
-        <v>102.5</v>
+        <v>102.2</v>
       </c>
       <c r="D57">
-        <v>106.5</v>
+        <v>105.9</v>
       </c>
       <c r="E57">
-        <v>99.7</v>
+        <v>99.3</v>
       </c>
     </row>
     <row r="58">
@@ -11077,13 +11419,13 @@
         <v>43709</v>
       </c>
       <c r="C58">
-        <v>102.9</v>
+        <v>102.6</v>
       </c>
       <c r="D58">
-        <v>103.9</v>
+        <v>103.4</v>
       </c>
       <c r="E58">
-        <v>98.2</v>
+        <v>97.8</v>
       </c>
     </row>
     <row r="59">
@@ -11096,13 +11438,13 @@
         <v>43739</v>
       </c>
       <c r="C59">
-        <v>103.2</v>
+        <v>102.9</v>
       </c>
       <c r="D59">
-        <v>103</v>
+        <v>102.6</v>
       </c>
       <c r="E59">
-        <v>95.7</v>
+        <v>95.3</v>
       </c>
     </row>
     <row r="60">
@@ -11115,13 +11457,13 @@
         <v>43770</v>
       </c>
       <c r="C60">
-        <v>104.8</v>
+        <v>104.5</v>
       </c>
       <c r="D60">
-        <v>103.3</v>
+        <v>102.9</v>
       </c>
       <c r="E60">
-        <v>99.59999999999999</v>
+        <v>99.2</v>
       </c>
     </row>
     <row r="61">
@@ -11134,13 +11476,13 @@
         <v>43800</v>
       </c>
       <c r="C61">
-        <v>102.8</v>
+        <v>102.5</v>
       </c>
       <c r="D61">
-        <v>102.8</v>
+        <v>102.3</v>
       </c>
       <c r="E61">
-        <v>100.9</v>
+        <v>100.4</v>
       </c>
     </row>
     <row r="62">
@@ -11153,13 +11495,13 @@
         <v>43831</v>
       </c>
       <c r="C62">
-        <v>103.7</v>
+        <v>103.4</v>
       </c>
       <c r="D62">
-        <v>105</v>
+        <v>104.6</v>
       </c>
       <c r="E62">
-        <v>101.1</v>
+        <v>100.6</v>
       </c>
     </row>
     <row r="63">
@@ -11172,13 +11514,13 @@
         <v>43862</v>
       </c>
       <c r="C63">
-        <v>101.7</v>
+        <v>101.4</v>
       </c>
       <c r="D63">
-        <v>106.4</v>
+        <v>105.8</v>
       </c>
       <c r="E63">
-        <v>100.5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64">
@@ -11191,13 +11533,13 @@
         <v>43891</v>
       </c>
       <c r="C64">
-        <v>93.90000000000001</v>
+        <v>93.59999999999999</v>
       </c>
       <c r="D64">
-        <v>101.1</v>
+        <v>100.7</v>
       </c>
       <c r="E64">
-        <v>96.3</v>
+        <v>95.8</v>
       </c>
     </row>
     <row r="65">
@@ -11210,13 +11552,13 @@
         <v>43922</v>
       </c>
       <c r="C65">
-        <v>79.09999999999999</v>
+        <v>78.8</v>
       </c>
       <c r="D65">
         <v>69.40000000000001</v>
       </c>
       <c r="E65">
-        <v>74.3</v>
+        <v>74.2</v>
       </c>
     </row>
     <row r="66">
@@ -11229,13 +11571,13 @@
         <v>43952</v>
       </c>
       <c r="C66">
-        <v>82.09999999999999</v>
+        <v>81.8</v>
       </c>
       <c r="D66">
-        <v>79</v>
+        <v>78.90000000000001</v>
       </c>
       <c r="E66">
-        <v>80</v>
+        <v>79.7</v>
       </c>
     </row>
     <row r="67">
@@ -11248,13 +11590,13 @@
         <v>43983</v>
       </c>
       <c r="C67">
-        <v>89.3</v>
+        <v>89</v>
       </c>
       <c r="D67">
-        <v>88.5</v>
+        <v>88.3</v>
       </c>
       <c r="E67">
-        <v>84.09999999999999</v>
+        <v>83.8</v>
       </c>
     </row>
     <row r="68">
@@ -11267,13 +11609,13 @@
         <v>44013</v>
       </c>
       <c r="C68">
-        <v>90.2</v>
+        <v>89.90000000000001</v>
       </c>
       <c r="D68">
-        <v>92</v>
+        <v>91.7</v>
       </c>
       <c r="E68">
-        <v>88.90000000000001</v>
+        <v>88.59999999999999</v>
       </c>
     </row>
     <row r="69">
@@ -11286,13 +11628,13 @@
         <v>44044</v>
       </c>
       <c r="C69">
-        <v>94.40000000000001</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="D69">
-        <v>91.40000000000001</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="E69">
-        <v>89</v>
+        <v>88.7</v>
       </c>
     </row>
     <row r="70">
@@ -11305,13 +11647,13 @@
         <v>44075</v>
       </c>
       <c r="C70">
-        <v>96</v>
+        <v>95.7</v>
       </c>
       <c r="D70">
-        <v>88.90000000000001</v>
+        <v>88.59999999999999</v>
       </c>
       <c r="E70">
-        <v>91.7</v>
+        <v>91.3</v>
       </c>
     </row>
     <row r="71">
@@ -11324,13 +11666,13 @@
         <v>44105</v>
       </c>
       <c r="C71">
-        <v>96.40000000000001</v>
+        <v>96.09999999999999</v>
       </c>
       <c r="D71">
-        <v>84.3</v>
+        <v>84</v>
       </c>
       <c r="E71">
-        <v>94.3</v>
+        <v>93.8</v>
       </c>
     </row>
     <row r="72">
@@ -11343,13 +11685,13 @@
         <v>44136</v>
       </c>
       <c r="C72">
-        <v>96.8</v>
+        <v>96.5</v>
       </c>
       <c r="D72">
-        <v>88.09999999999999</v>
+        <v>87.8</v>
       </c>
       <c r="E72">
-        <v>94.40000000000001</v>
+        <v>93.90000000000001</v>
       </c>
     </row>
     <row r="73">
@@ -11362,13 +11704,13 @@
         <v>44166</v>
       </c>
       <c r="C73">
-        <v>94</v>
+        <v>93.7</v>
       </c>
       <c r="D73">
-        <v>87.5</v>
+        <v>87.09999999999999</v>
       </c>
       <c r="E73">
-        <v>96.8</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="74">
@@ -11381,13 +11723,13 @@
         <v>44197</v>
       </c>
       <c r="C74">
-        <v>92</v>
+        <v>91.7</v>
       </c>
       <c r="D74">
-        <v>93.7</v>
+        <v>93.2</v>
       </c>
       <c r="E74">
-        <v>98.09999999999999</v>
+        <v>97.40000000000001</v>
       </c>
     </row>
     <row r="75">
@@ -11400,13 +11742,13 @@
         <v>44228</v>
       </c>
       <c r="C75">
-        <v>91.90000000000001</v>
+        <v>91.5</v>
       </c>
       <c r="D75">
-        <v>97.5</v>
+        <v>97</v>
       </c>
       <c r="E75">
-        <v>100.7</v>
+        <v>99.90000000000001</v>
       </c>
     </row>
     <row r="76">
@@ -11419,13 +11761,13 @@
         <v>44256</v>
       </c>
       <c r="C76">
-        <v>100.2</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="D76">
-        <v>93.90000000000001</v>
+        <v>93.3</v>
       </c>
       <c r="E76">
-        <v>101.2</v>
+        <v>100.5</v>
       </c>
     </row>
     <row r="77">
@@ -11438,13 +11780,13 @@
         <v>44287</v>
       </c>
       <c r="C77">
-        <v>104.5</v>
+        <v>104.1</v>
       </c>
       <c r="D77">
-        <v>108.4</v>
+        <v>107.6</v>
       </c>
       <c r="E77">
-        <v>113.1</v>
+        <v>112.2</v>
       </c>
     </row>
     <row r="78">
@@ -11457,13 +11799,13 @@
         <v>44317</v>
       </c>
       <c r="C78">
-        <v>107.3</v>
+        <v>106.9</v>
       </c>
       <c r="D78">
-        <v>110.8</v>
+        <v>110</v>
       </c>
       <c r="E78">
-        <v>112.6</v>
+        <v>111.8</v>
       </c>
     </row>
     <row r="79">
@@ -11476,13 +11818,13 @@
         <v>44348</v>
       </c>
       <c r="C79">
-        <v>112.5</v>
+        <v>112.1</v>
       </c>
       <c r="D79">
-        <v>112.3</v>
+        <v>111.4</v>
       </c>
       <c r="E79">
-        <v>113.5</v>
+        <v>112.6</v>
       </c>
     </row>
     <row r="80">
@@ -11495,13 +11837,13 @@
         <v>44378</v>
       </c>
       <c r="C80">
-        <v>110.6</v>
+        <v>110.2</v>
       </c>
       <c r="D80">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E80">
-        <v>113.5</v>
+        <v>112.6</v>
       </c>
     </row>
     <row r="81">
@@ -11514,13 +11856,13 @@
         <v>44409</v>
       </c>
       <c r="C81">
+        <v>113.1</v>
+      </c>
+      <c r="D81">
+        <v>110</v>
+      </c>
+      <c r="E81">
         <v>113.5</v>
-      </c>
-      <c r="D81">
-        <v>111</v>
-      </c>
-      <c r="E81">
-        <v>114.5</v>
       </c>
     </row>
     <row r="82">
@@ -11533,13 +11875,13 @@
         <v>44440</v>
       </c>
       <c r="C82">
-        <v>114.4</v>
+        <v>114</v>
       </c>
       <c r="D82">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E82">
-        <v>115.7</v>
+        <v>114.6</v>
       </c>
     </row>
     <row r="83">
@@ -11552,13 +11894,70 @@
         <v>44470</v>
       </c>
       <c r="C83">
-        <v>112.8</v>
+        <v>112.4</v>
       </c>
       <c r="D83">
-        <v>117.7</v>
+        <v>116.8</v>
       </c>
       <c r="E83">
-        <v>119.7</v>
+        <v>118.6</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>The Employment expectations indicator is a composite measure (average = 100)</t>
+        </is>
+      </c>
+      <c r="B84" s="2">
+        <v>44501</v>
+      </c>
+      <c r="C84">
+        <v>113</v>
+      </c>
+      <c r="D84">
+        <v>117.4</v>
+      </c>
+      <c r="E84">
+        <v>118.2</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>The Employment expectations indicator is a composite measure (average = 100)</t>
+        </is>
+      </c>
+      <c r="B85" s="2">
+        <v>44531</v>
+      </c>
+      <c r="C85">
+        <v>112.3</v>
+      </c>
+      <c r="D85">
+        <v>118.9</v>
+      </c>
+      <c r="E85">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>The Employment expectations indicator is a composite measure (average = 100)</t>
+        </is>
+      </c>
+      <c r="B86" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C86">
+        <v>112.1</v>
+      </c>
+      <c r="D86">
+        <v>110.9</v>
+      </c>
+      <c r="E86">
+        <v>114.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>